<commit_message>
Added both 'file_renamer.py' and 'file_predictor_leaveout.cmd' and modified 'model_predictor.py' to work properly with 'file_predictor_leaveout.cmd'.
</commit_message>
<xml_diff>
--- a/project_files/documentation/model_shapes.xlsx
+++ b/project_files/documentation/model_shapes.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D207"/>
+  <dimension ref="A1:D208"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4508,6 +4508,26 @@
         <v>60</v>
       </c>
     </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added another script explanation for 'ext_raw_measures.py', added 'data_balancer.py' script, modified 'rnn.py' and 'model_predictor.py' to work with balanced datasets, and refactored 'graph_creator.py' and added other function to plot single act plots.
</commit_message>
<xml_diff>
--- a/project_files/documentation/model_shapes.xlsx
+++ b/project_files/documentation/model_shapes.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D223"/>
+  <dimension ref="A1:D240"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4828,6 +4828,346 @@
         <v>10</v>
       </c>
     </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D224" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D225" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D226" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D227" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D228" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D229" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D230" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D231" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D232" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D233" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D234" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>jointAngleXZY</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D235" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>jointAngleXZY</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D236" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>jointAngleXZY</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D237" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D238" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D239" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D240" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added another script explanation and minor changes made to other scripts to enable 'allmatfiles' to be used to train/test.
</commit_message>
<xml_diff>
--- a/project_files/documentation/model_shapes.xlsx
+++ b/project_files/documentation/model_shapes.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D240"/>
+  <dimension ref="A1:D276"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5168,6 +5168,726 @@
         <v>10</v>
       </c>
     </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D241" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D242" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D243" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D244" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D245" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D246" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D247" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D248" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D249" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D250" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D251" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D252" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>jointAngleXZY</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D253" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>jointAngleXZY</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>jointAngleXZY</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>sensorMagneticField</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>jointAngleXZY</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D268" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>jointAngleXZY</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>jointAngleXZY</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>allmatfiles</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>jointAngle</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified 'ft_sel_red' and 'mat_act_div' to have additional optional args, changed 'rnn', 'model_predictor', 'comp_stat_vals', and 'ext_raw_measures' to make use of these args, added ability of 'rnn' to preprocess the cnn dataset, and added 'predictions_selector'.
</commit_message>
<xml_diff>
--- a/project_files/documentation/model_shapes.xlsx
+++ b/project_files/documentation/model_shapes.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D276"/>
+  <dimension ref="A1:D285"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5888,6 +5888,186 @@
         <v>60</v>
       </c>
     </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>position</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>dhc</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>overall</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>NSAA</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>AD</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>acts</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>